<commit_message>
Preparing the update to the QRDA category 1 validation checklist
</commit_message>
<xml_diff>
--- a/documents/cypress_ep_qrda_category_1_validation_checklist_05132013.xlsx
+++ b/documents/cypress_ep_qrda_category_1_validation_checklist_05132013.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="2320" windowWidth="39840" windowHeight="27140" tabRatio="988"/>
+    <workbookView xWindow="23960" yWindow="3180" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions (2)" sheetId="201" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="101" r:id="rId1"/>
     <sheet name="0002" sheetId="1" r:id="rId2"/>
     <sheet name="0004a" sheetId="2" r:id="rId3"/>
     <sheet name="0004b" sheetId="3" r:id="rId4"/>
@@ -108,105 +108,6 @@
     <sheet name="PrimaryCariesPreventionb" sheetId="98" r:id="rId99"/>
     <sheet name="PrimaryCariesPreventionc" sheetId="99" r:id="rId100"/>
     <sheet name="PrimaryCariesPreventiond" sheetId="100" r:id="rId101"/>
-    <sheet name="Sheet2" sheetId="102" r:id="rId102"/>
-    <sheet name="Sheet3" sheetId="103" r:id="rId103"/>
-    <sheet name="Sheet4" sheetId="104" r:id="rId104"/>
-    <sheet name="Sheet5" sheetId="105" r:id="rId105"/>
-    <sheet name="Sheet6" sheetId="106" r:id="rId106"/>
-    <sheet name="Sheet7" sheetId="107" r:id="rId107"/>
-    <sheet name="Sheet8" sheetId="108" r:id="rId108"/>
-    <sheet name="Sheet9" sheetId="109" r:id="rId109"/>
-    <sheet name="Sheet10" sheetId="110" r:id="rId110"/>
-    <sheet name="Sheet11" sheetId="111" r:id="rId111"/>
-    <sheet name="Sheet12" sheetId="112" r:id="rId112"/>
-    <sheet name="Sheet13" sheetId="113" r:id="rId113"/>
-    <sheet name="Sheet14" sheetId="114" r:id="rId114"/>
-    <sheet name="Sheet15" sheetId="115" r:id="rId115"/>
-    <sheet name="Sheet16" sheetId="116" r:id="rId116"/>
-    <sheet name="Sheet17" sheetId="117" r:id="rId117"/>
-    <sheet name="Sheet18" sheetId="118" r:id="rId118"/>
-    <sheet name="Sheet19" sheetId="119" r:id="rId119"/>
-    <sheet name="Sheet20" sheetId="120" r:id="rId120"/>
-    <sheet name="Sheet21" sheetId="121" r:id="rId121"/>
-    <sheet name="Sheet22" sheetId="122" r:id="rId122"/>
-    <sheet name="Sheet23" sheetId="123" r:id="rId123"/>
-    <sheet name="Sheet24" sheetId="124" r:id="rId124"/>
-    <sheet name="Sheet25" sheetId="125" r:id="rId125"/>
-    <sheet name="Sheet26" sheetId="126" r:id="rId126"/>
-    <sheet name="Sheet27" sheetId="127" r:id="rId127"/>
-    <sheet name="Sheet28" sheetId="128" r:id="rId128"/>
-    <sheet name="Sheet29" sheetId="129" r:id="rId129"/>
-    <sheet name="Sheet30" sheetId="130" r:id="rId130"/>
-    <sheet name="Sheet31" sheetId="131" r:id="rId131"/>
-    <sheet name="Sheet32" sheetId="132" r:id="rId132"/>
-    <sheet name="Sheet33" sheetId="133" r:id="rId133"/>
-    <sheet name="Sheet34" sheetId="134" r:id="rId134"/>
-    <sheet name="Sheet35" sheetId="135" r:id="rId135"/>
-    <sheet name="Sheet36" sheetId="136" r:id="rId136"/>
-    <sheet name="Sheet37" sheetId="137" r:id="rId137"/>
-    <sheet name="Sheet38" sheetId="138" r:id="rId138"/>
-    <sheet name="Sheet39" sheetId="139" r:id="rId139"/>
-    <sheet name="Sheet40" sheetId="140" r:id="rId140"/>
-    <sheet name="Sheet41" sheetId="141" r:id="rId141"/>
-    <sheet name="Sheet42" sheetId="142" r:id="rId142"/>
-    <sheet name="Sheet43" sheetId="143" r:id="rId143"/>
-    <sheet name="Sheet44" sheetId="144" r:id="rId144"/>
-    <sheet name="Sheet45" sheetId="145" r:id="rId145"/>
-    <sheet name="Sheet46" sheetId="146" r:id="rId146"/>
-    <sheet name="Sheet47" sheetId="147" r:id="rId147"/>
-    <sheet name="Sheet48" sheetId="148" r:id="rId148"/>
-    <sheet name="Sheet49" sheetId="149" r:id="rId149"/>
-    <sheet name="Sheet50" sheetId="150" r:id="rId150"/>
-    <sheet name="Sheet51" sheetId="151" r:id="rId151"/>
-    <sheet name="Sheet52" sheetId="152" r:id="rId152"/>
-    <sheet name="Sheet53" sheetId="153" r:id="rId153"/>
-    <sheet name="Sheet54" sheetId="154" r:id="rId154"/>
-    <sheet name="Sheet55" sheetId="155" r:id="rId155"/>
-    <sheet name="Sheet56" sheetId="156" r:id="rId156"/>
-    <sheet name="Sheet57" sheetId="157" r:id="rId157"/>
-    <sheet name="Sheet58" sheetId="158" r:id="rId158"/>
-    <sheet name="Sheet59" sheetId="159" r:id="rId159"/>
-    <sheet name="Sheet60" sheetId="160" r:id="rId160"/>
-    <sheet name="Sheet61" sheetId="161" r:id="rId161"/>
-    <sheet name="Sheet62" sheetId="162" r:id="rId162"/>
-    <sheet name="Sheet63" sheetId="163" r:id="rId163"/>
-    <sheet name="Sheet64" sheetId="164" r:id="rId164"/>
-    <sheet name="Sheet65" sheetId="165" r:id="rId165"/>
-    <sheet name="Sheet66" sheetId="166" r:id="rId166"/>
-    <sheet name="Sheet67" sheetId="167" r:id="rId167"/>
-    <sheet name="Sheet68" sheetId="168" r:id="rId168"/>
-    <sheet name="Sheet69" sheetId="169" r:id="rId169"/>
-    <sheet name="Sheet70" sheetId="170" r:id="rId170"/>
-    <sheet name="Sheet71" sheetId="171" r:id="rId171"/>
-    <sheet name="Sheet72" sheetId="172" r:id="rId172"/>
-    <sheet name="Sheet73" sheetId="173" r:id="rId173"/>
-    <sheet name="Sheet74" sheetId="174" r:id="rId174"/>
-    <sheet name="Sheet75" sheetId="175" r:id="rId175"/>
-    <sheet name="Sheet76" sheetId="176" r:id="rId176"/>
-    <sheet name="Sheet77" sheetId="177" r:id="rId177"/>
-    <sheet name="Sheet78" sheetId="178" r:id="rId178"/>
-    <sheet name="Sheet79" sheetId="179" r:id="rId179"/>
-    <sheet name="Sheet80" sheetId="180" r:id="rId180"/>
-    <sheet name="Sheet81" sheetId="181" r:id="rId181"/>
-    <sheet name="Sheet82" sheetId="182" r:id="rId182"/>
-    <sheet name="Sheet83" sheetId="183" r:id="rId183"/>
-    <sheet name="Sheet84" sheetId="184" r:id="rId184"/>
-    <sheet name="Sheet85" sheetId="185" r:id="rId185"/>
-    <sheet name="Sheet86" sheetId="186" r:id="rId186"/>
-    <sheet name="Sheet87" sheetId="187" r:id="rId187"/>
-    <sheet name="Sheet88" sheetId="188" r:id="rId188"/>
-    <sheet name="Sheet89" sheetId="189" r:id="rId189"/>
-    <sheet name="Sheet90" sheetId="190" r:id="rId190"/>
-    <sheet name="Sheet91" sheetId="191" r:id="rId191"/>
-    <sheet name="Sheet92" sheetId="192" r:id="rId192"/>
-    <sheet name="Sheet93" sheetId="193" r:id="rId193"/>
-    <sheet name="Sheet94" sheetId="194" r:id="rId194"/>
-    <sheet name="Sheet95" sheetId="195" r:id="rId195"/>
-    <sheet name="Sheet96" sheetId="196" r:id="rId196"/>
-    <sheet name="Sheet97" sheetId="197" r:id="rId197"/>
-    <sheet name="Sheet98" sheetId="198" r:id="rId198"/>
-    <sheet name="Sheet99" sheetId="199" r:id="rId199"/>
-    <sheet name="Sheet100" sheetId="200" r:id="rId200"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -472,7 +373,7 @@
     <t>2.16.840.1.113883.3.526.3.1170</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.10.20.24.3.101</t>
+    <t>2.16.840.1.113883.10.20.22.4.85</t>
   </si>
   <si>
     <t>Heart_Adult_C</t>
@@ -1427,7 +1328,7 @@
         <sz val="10"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>The patient names generated by Cypress are randomly assigned to the records before they are presented from Cypress to an EHR system.  In order to translate the  short-hand names that are provide in this Cypress QRDA Category 1 Validation Checklist document, you will need to identify the "Name" from the data presented by the EHR associated with the QRDA Category 1 XML</t>
+      <t>The patient names generated by Cypress are randomly assigned to the records before they are presented from Cypress to an EHR system.  In order to translate the the short-hand names that are provide in this Cypress QRDA Category 1 Validation Checklist document, you will need to identify the "Name" from the data presented by the EHR associated with the QRDA Category 1 XML</t>
     </r>
   </si>
   <si>
@@ -1438,14 +1339,14 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>Step 3</t>
+      <t>Step 3:</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>: For each patient uploaded into Cypress for each specific CQM, visually bring up the QRDA Category 1 XML associated with that patient in Cypress, and perform a "Find" for the "Template ID" of that patient in the QRDA Category 1 XML.  The "Template IDs" that should match that patient are enumerated in the Cypress QRDA Category 1 Validation Checklist using the tabs in the spreadsheet to navigate to the CQM definition, and are located under column "D" after each patient named in the Cypress QRDA Category 1 Validation Checklist.</t>
+      <t xml:space="preserve"> For each patient uploaded into Cypress for each specific CQM, visually bring up the QRDA Category 1 XML associated with that patient in Cypress, and perform a "Find" for the "Template ID" of that patient in the QRDA Category 1 XML.  The "Template IDs" that should match that patient are enumerated in the Cypress QRDA Category 1 Validation Checklist using the tabs in the spreadsheet to navigate to the CQM definition, and are located under column "D" after each patient named in the Cypress QRDA Category 1 Validation Checklist.</t>
     </r>
   </si>
   <si>
@@ -1456,14 +1357,7 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>Step 4:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">Step 4: </t>
     </r>
     <r>
       <rPr>
@@ -1532,7 +1426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1541,9 +1435,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1561,101 +1452,200 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>43180</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>469900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7399181</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1617979</xdr:rowOff>
+      <xdr:colOff>7366000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1668780</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Screen Shot 2013-04-26 at 11.27.55 AM.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="0" y="3078480"/>
-          <a:ext cx="7399181" cy="1574799"/>
+          <a:off x="0" y="10782300"/>
+          <a:ext cx="7366000" cy="1681480"/>
+          <a:chOff x="0" y="10947400"/>
+          <a:chExt cx="7366000" cy="1681480"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="Picture 2" descr="Screen Shot 2013-04-26 at 12.00.29 PM.png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="10960100"/>
+            <a:ext cx="7366000" cy="1600200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rounded Rectangle 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4254500" y="10947400"/>
+            <a:ext cx="1617980" cy="1681480"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1391921</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>762000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2095501</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1541780</xdr:rowOff>
+      <xdr:colOff>7366000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1617980</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rounded Rectangle 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="5" name="Group 4"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1391921" y="3035300"/>
-          <a:ext cx="703580" cy="1541780"/>
+          <a:off x="0" y="8470900"/>
+          <a:ext cx="7366000" cy="1681480"/>
+          <a:chOff x="0" y="8636000"/>
+          <a:chExt cx="7366000" cy="1681480"/>
         </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="31750">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="6" name="Picture 5" descr="Screen Shot 2013-04-26 at 12.00.29 PM.png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="8699500"/>
+            <a:ext cx="7366000" cy="1600200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Rounded Rectangle 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5740400" y="8636000"/>
+            <a:ext cx="1617980" cy="1681480"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -1671,294 +1661,191 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>2032000</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Screen Shot 2013-04-26 at 11.18.24 AM.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="5613400"/>
           <a:ext cx="7399547" cy="2032000"/>
+          <a:chOff x="0" y="5778500"/>
+          <a:chExt cx="7399547" cy="2032000"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>185420</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>744220</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1803400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1567180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rounded Rectangle 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="185420" y="6357620"/>
-          <a:ext cx="1617980" cy="822960"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="31750">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="9" name="Picture 8" descr="Screen Shot 2013-04-26 at 11.18.24 AM.png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="5778500"/>
+            <a:ext cx="7399547" cy="2032000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rounded Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="165100" y="6565900"/>
+            <a:ext cx="1617980" cy="822960"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>5080</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7366000</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1605280</xdr:rowOff>
+      <xdr:colOff>7399181</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1701799</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="Screen Shot 2013-04-26 at 12.00.29 PM.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="11" name="Group 10"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="0" y="8615680"/>
-          <a:ext cx="7366000" cy="1600200"/>
+          <a:off x="0" y="3060700"/>
+          <a:ext cx="7399181" cy="1612899"/>
+          <a:chOff x="0" y="3060700"/>
+          <a:chExt cx="7399181" cy="1612899"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5709920</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7327900</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1681480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rounded Rectangle 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5709920" y="8610600"/>
-          <a:ext cx="1617980" cy="1681480"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="31750">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>5080</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7366000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>81280</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="Screen Shot 2013-04-26 at 12.00.29 PM.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="10876280"/>
-          <a:ext cx="7366000" cy="1600200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4274820</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>482600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5892800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rounded Rectangle 8"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4274820" y="10858500"/>
-          <a:ext cx="1617980" cy="1625600"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="31750">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="12" name="Picture 11" descr="Screen Shot 2013-04-26 at 11.27.55 AM.png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="3098800"/>
+            <a:ext cx="7399181" cy="1574799"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rounded Rectangle 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1371600" y="3060700"/>
+            <a:ext cx="703580" cy="1541780"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2284,58 +2171,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="84" customWidth="1"/>
+    <col min="1" max="1" width="84.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="66" customHeight="1">
+    <row r="1" spans="1:1" ht="65">
       <c r="A1" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="66" customHeight="1">
+    <row r="2" spans="1:1" ht="65">
       <c r="A2" s="2" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="52" customHeight="1">
+    <row r="3" spans="1:1" ht="52">
       <c r="A3" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="55" customHeight="1">
+    <row r="4" spans="1:1" ht="52">
       <c r="A4" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="134" customHeight="1"/>
-    <row r="6" spans="1:1" ht="69" customHeight="1">
+    <row r="5" spans="1:1" ht="143" customHeight="1">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:1" ht="65">
       <c r="A6" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="167" customHeight="1"/>
-    <row r="8" spans="1:1" ht="69" customHeight="1">
+    <row r="7" spans="1:1" ht="165" customHeight="1">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:1" ht="65">
       <c r="A8" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="139" customHeight="1"/>
-    <row r="10" spans="1:1" ht="39" customHeight="1">
-      <c r="A10" s="4" t="s">
+    <row r="9" spans="1:1" ht="140" customHeight="1">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:1" ht="38" customHeight="1">
+      <c r="A10" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="120" customHeight="1"/>
-    <row r="13" spans="1:1" ht="73" customHeight="1">
-      <c r="A13" s="1" t="s">
+    <row r="11" spans="1:1" ht="134" customHeight="1">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:1" ht="65">
+      <c r="A12" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -2999,142 +2894,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet105.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet106.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet107.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet108.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet109.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
@@ -3318,176 +3077,6 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet110.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet111.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet112.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet113.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet114.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet115.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet116.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet117.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet118.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet119.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3888,176 +3477,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet120.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet121.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet122.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet123.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet124.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet125.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet126.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet127.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet128.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet129.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
@@ -4409,176 +3828,6 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet130.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet131.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet132.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet133.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet134.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet135.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet136.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet137.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet138.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet139.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4946,176 +4195,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet140.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet141.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet142.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet143.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet144.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet145.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet146.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet147.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet148.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet149.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
@@ -5337,176 +4416,6 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet150.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet151.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet152.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet153.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet154.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet155.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet156.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet157.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet158.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet159.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5712,176 +4621,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet160.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet161.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet162.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet163.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet164.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet165.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet166.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet167.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet168.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet169.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
@@ -6103,176 +4842,6 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet170.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet171.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet172.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet173.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet174.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet175.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet176.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet177.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet178.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet179.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6445,176 +5014,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet180.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet181.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet182.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet183.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet184.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet185.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet186.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet187.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet188.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet189.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
@@ -6844,181 +5243,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet190.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet191.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet192.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet193.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet194.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet195.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet196.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet197.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet198.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet199.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
@@ -7381,23 +5610,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet200.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>

</xml_diff>